<commit_message>
add validation to title check
</commit_message>
<xml_diff>
--- a/config_portal/examples/images-example.xlsx
+++ b/config_portal/examples/images-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/HuBMAP-pancreas-data-explorer/HuBMAP-pancreas-data-explorer/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/HuBMAP-pancreas-data-explorer/HuBMAP-pancreas-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F5CB96-F468-BA42-8C93-41A0DE832B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A09AF9-8A6B-D440-9686-582B86C8CFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="2960" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
+    <workbookView xWindow="2300" yWindow="3280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
   </bookViews>
   <sheets>
     <sheet name="block-data" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Order</t>
   </si>
   <si>
-    <t>Block ID</t>
-  </si>
-  <si>
     <t>Anatomical region</t>
   </si>
   <si>
@@ -670,6 +667,9 @@
   </si>
   <si>
     <t>Channels</t>
+  </si>
+  <si>
+    <t>Tissue Block</t>
   </si>
 </sst>
 </file>
@@ -1084,59 +1084,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -1161,16 +1161,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1178,16 +1178,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1195,16 +1195,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1212,16 +1212,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1229,16 +1229,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1246,16 +1246,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1263,16 +1263,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1280,16 +1280,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1308,49 +1308,49 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>210</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E2">
         <v>2048</v>
@@ -1367,13 +1367,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3">
@@ -1391,13 +1391,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4">
@@ -1415,13 +1415,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5">
@@ -1439,13 +1439,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6">
@@ -1463,13 +1463,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7">
@@ -1487,13 +1487,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8">
@@ -1511,13 +1511,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9">
@@ -1535,13 +1535,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10">
@@ -1559,13 +1559,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11">
@@ -1583,13 +1583,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12">
@@ -1607,13 +1607,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13">
@@ -1631,13 +1631,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14">
@@ -1655,13 +1655,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
         <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15">
@@ -1679,13 +1679,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>51</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16">
@@ -1703,13 +1703,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17">
@@ -1727,13 +1727,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
         <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>55</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18">
@@ -1751,13 +1751,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19">
@@ -1775,13 +1775,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20">
@@ -1799,13 +1799,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21">
@@ -1823,13 +1823,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
         <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22">
@@ -1847,13 +1847,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
         <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23">
@@ -1871,13 +1871,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24">
@@ -1895,13 +1895,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
         <v>68</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25">
@@ -1919,13 +1919,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
         <v>70</v>
-      </c>
-      <c r="C26" t="s">
-        <v>71</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26">
@@ -1943,13 +1943,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
         <v>72</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27">
@@ -1967,13 +1967,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" t="s">
         <v>74</v>
-      </c>
-      <c r="C28" t="s">
-        <v>75</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28">
@@ -1991,13 +1991,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
         <v>76</v>
-      </c>
-      <c r="C29" t="s">
-        <v>77</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29">
@@ -2015,13 +2015,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
         <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>79</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30">
@@ -2039,13 +2039,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
         <v>80</v>
-      </c>
-      <c r="C31" t="s">
-        <v>81</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31">
@@ -2063,13 +2063,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" t="s">
         <v>82</v>
-      </c>
-      <c r="C32" t="s">
-        <v>83</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32">
@@ -2087,13 +2087,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
         <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>85</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33">
@@ -2111,13 +2111,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
         <v>86</v>
-      </c>
-      <c r="C34" t="s">
-        <v>87</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34">
@@ -2135,13 +2135,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
         <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>89</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35">
@@ -2159,13 +2159,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
         <v>90</v>
-      </c>
-      <c r="C36" t="s">
-        <v>91</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36">
@@ -2183,13 +2183,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
         <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>93</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37">
@@ -2207,13 +2207,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
         <v>94</v>
-      </c>
-      <c r="C38" t="s">
-        <v>95</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38">
@@ -2231,13 +2231,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" t="s">
         <v>96</v>
-      </c>
-      <c r="C39" t="s">
-        <v>97</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39">
@@ -2255,13 +2255,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
         <v>98</v>
-      </c>
-      <c r="C40" t="s">
-        <v>99</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40">
@@ -2279,13 +2279,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
         <v>100</v>
-      </c>
-      <c r="C41" t="s">
-        <v>101</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41">
@@ -2303,13 +2303,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" t="s">
         <v>102</v>
-      </c>
-      <c r="C42" t="s">
-        <v>103</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42">
@@ -2327,13 +2327,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" t="s">
         <v>104</v>
-      </c>
-      <c r="C43" t="s">
-        <v>105</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43">
@@ -2351,13 +2351,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
         <v>106</v>
-      </c>
-      <c r="C44" t="s">
-        <v>107</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44">
@@ -2375,13 +2375,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
         <v>108</v>
-      </c>
-      <c r="C45" t="s">
-        <v>109</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45">
@@ -2399,13 +2399,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" t="s">
         <v>110</v>
-      </c>
-      <c r="C46" t="s">
-        <v>111</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46">
@@ -2423,13 +2423,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
         <v>112</v>
-      </c>
-      <c r="C47" t="s">
-        <v>113</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47">
@@ -2447,13 +2447,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" t="s">
         <v>114</v>
-      </c>
-      <c r="C48" t="s">
-        <v>115</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48">
@@ -2471,13 +2471,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" t="s">
         <v>116</v>
-      </c>
-      <c r="C49" t="s">
-        <v>117</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49">
@@ -2495,13 +2495,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" t="s">
         <v>118</v>
-      </c>
-      <c r="C50" t="s">
-        <v>119</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50">
@@ -2519,13 +2519,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" t="s">
         <v>120</v>
-      </c>
-      <c r="C51" t="s">
-        <v>121</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51">
@@ -2543,13 +2543,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" t="s">
         <v>122</v>
-      </c>
-      <c r="C52" t="s">
-        <v>123</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52">
@@ -2567,13 +2567,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53" t="s">
         <v>124</v>
-      </c>
-      <c r="C53" t="s">
-        <v>125</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53">
@@ -2591,13 +2591,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" t="s">
         <v>126</v>
-      </c>
-      <c r="C54" t="s">
-        <v>127</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54">
@@ -2615,13 +2615,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" t="s">
         <v>128</v>
-      </c>
-      <c r="C55" t="s">
-        <v>129</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55">
@@ -2639,13 +2639,13 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" t="s">
         <v>130</v>
-      </c>
-      <c r="C56" t="s">
-        <v>131</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56">
@@ -2663,13 +2663,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57" t="s">
         <v>132</v>
-      </c>
-      <c r="C57" t="s">
-        <v>133</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57">
@@ -2687,13 +2687,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
         <v>134</v>
-      </c>
-      <c r="C58" t="s">
-        <v>135</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58">
@@ -2711,13 +2711,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" t="s">
         <v>136</v>
-      </c>
-      <c r="C59" t="s">
-        <v>137</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59">
@@ -2735,13 +2735,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" t="s">
         <v>138</v>
-      </c>
-      <c r="C60" t="s">
-        <v>139</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60">
@@ -2759,13 +2759,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" t="s">
         <v>140</v>
-      </c>
-      <c r="C61" t="s">
-        <v>141</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61">
@@ -2783,13 +2783,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" t="s">
+        <v>141</v>
+      </c>
+      <c r="C62" t="s">
         <v>142</v>
-      </c>
-      <c r="C62" t="s">
-        <v>143</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62">
@@ -2807,13 +2807,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B63" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" t="s">
         <v>144</v>
-      </c>
-      <c r="C63" t="s">
-        <v>145</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63">
@@ -2831,13 +2831,13 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B64" t="s">
+        <v>145</v>
+      </c>
+      <c r="C64" t="s">
         <v>146</v>
-      </c>
-      <c r="C64" t="s">
-        <v>147</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64">
@@ -2855,13 +2855,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" t="s">
         <v>148</v>
-      </c>
-      <c r="C65" t="s">
-        <v>149</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65">
@@ -2879,13 +2879,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B66" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" t="s">
         <v>150</v>
-      </c>
-      <c r="C66" t="s">
-        <v>151</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66">
@@ -2903,13 +2903,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B67" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" t="s">
         <v>152</v>
-      </c>
-      <c r="C67" t="s">
-        <v>153</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67">
@@ -2927,13 +2927,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" t="s">
         <v>154</v>
-      </c>
-      <c r="C68" t="s">
-        <v>155</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68">
@@ -2951,13 +2951,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B69" t="s">
+        <v>155</v>
+      </c>
+      <c r="C69" t="s">
         <v>156</v>
-      </c>
-      <c r="C69" t="s">
-        <v>157</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69">
@@ -2975,13 +2975,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" t="s">
         <v>158</v>
-      </c>
-      <c r="C70" t="s">
-        <v>159</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70">
@@ -2999,13 +2999,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B71" t="s">
+        <v>159</v>
+      </c>
+      <c r="C71" t="s">
         <v>160</v>
-      </c>
-      <c r="C71" t="s">
-        <v>161</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71">
@@ -3023,13 +3023,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
+        <v>161</v>
+      </c>
+      <c r="C72" t="s">
         <v>162</v>
-      </c>
-      <c r="C72" t="s">
-        <v>163</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72">
@@ -3047,13 +3047,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" t="s">
         <v>164</v>
-      </c>
-      <c r="C73" t="s">
-        <v>165</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73">
@@ -3071,13 +3071,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" t="s">
         <v>166</v>
-      </c>
-      <c r="C74" t="s">
-        <v>167</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74">
@@ -3095,13 +3095,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" t="s">
         <v>168</v>
-      </c>
-      <c r="C75" t="s">
-        <v>169</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75">
@@ -3119,13 +3119,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" t="s">
         <v>170</v>
-      </c>
-      <c r="C76" t="s">
-        <v>171</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76">
@@ -3143,13 +3143,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
+        <v>171</v>
+      </c>
+      <c r="C77" t="s">
         <v>172</v>
-      </c>
-      <c r="C77" t="s">
-        <v>173</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77">
@@ -3167,13 +3167,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" t="s">
         <v>174</v>
-      </c>
-      <c r="C78" t="s">
-        <v>175</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78">
@@ -3191,13 +3191,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B79" t="s">
+        <v>175</v>
+      </c>
+      <c r="C79" t="s">
         <v>176</v>
-      </c>
-      <c r="C79" t="s">
-        <v>177</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79">
@@ -3215,13 +3215,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B80" t="s">
+        <v>177</v>
+      </c>
+      <c r="C80" t="s">
         <v>178</v>
-      </c>
-      <c r="C80" t="s">
-        <v>179</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80">
@@ -3239,13 +3239,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
+        <v>179</v>
+      </c>
+      <c r="C81" t="s">
         <v>180</v>
-      </c>
-      <c r="C81" t="s">
-        <v>181</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81">
@@ -3263,13 +3263,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B82" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82" t="s">
         <v>182</v>
-      </c>
-      <c r="C82" t="s">
-        <v>183</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82">
@@ -3287,13 +3287,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
+        <v>183</v>
+      </c>
+      <c r="C83" t="s">
         <v>184</v>
-      </c>
-      <c r="C83" t="s">
-        <v>185</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83">
@@ -3311,13 +3311,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B84" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" t="s">
         <v>186</v>
-      </c>
-      <c r="C84" t="s">
-        <v>187</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84">
@@ -3335,13 +3335,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" t="s">
         <v>188</v>
-      </c>
-      <c r="C85" t="s">
-        <v>189</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85">
@@ -3359,13 +3359,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B86" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" t="s">
         <v>190</v>
-      </c>
-      <c r="C86" t="s">
-        <v>191</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86">
@@ -3383,13 +3383,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B87" t="s">
+        <v>191</v>
+      </c>
+      <c r="C87" t="s">
         <v>192</v>
-      </c>
-      <c r="C87" t="s">
-        <v>193</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87">
@@ -3407,13 +3407,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B88" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" t="s">
         <v>194</v>
-      </c>
-      <c r="C88" t="s">
-        <v>195</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88">
@@ -3431,13 +3431,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B89" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" t="s">
         <v>196</v>
-      </c>
-      <c r="C89" t="s">
-        <v>197</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89">
@@ -3455,13 +3455,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B90" t="s">
+        <v>197</v>
+      </c>
+      <c r="C90" t="s">
         <v>198</v>
-      </c>
-      <c r="C90" t="s">
-        <v>199</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90">

</xml_diff>

<commit_message>
generalize names for scientific images display
</commit_message>
<xml_diff>
--- a/config_portal/examples/images-example.xlsx
+++ b/config_portal/examples/images-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/HuBMAP-pancreas-data-explorer/HuBMAP-pancreas-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A09AF9-8A6B-D440-9686-582B86C8CFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E499C9-D78E-724D-95DF-A4C6AB75045F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="3280" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
+    <workbookView xWindow="3060" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
   </bookViews>
   <sheets>
     <sheet name="block-data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
   <si>
     <t>Order</t>
   </si>
@@ -670,6 +670,12 @@
   </si>
   <si>
     <t>Tissue Block</t>
+  </si>
+  <si>
+    <t>Optical Clearing</t>
+  </si>
+  <si>
+    <t>Image Category</t>
   </si>
 </sst>
 </file>
@@ -1305,15 +1311,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A62E87D-1C39-EA44-B778-5ACEBBC062C4}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>210</v>
       </c>
@@ -1321,25 +1327,28 @@
         <v>203</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1347,25 +1356,28 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="E2">
-        <v>2048</v>
       </c>
       <c r="F2">
         <v>2048</v>
       </c>
       <c r="G2">
+        <v>2048</v>
+      </c>
+      <c r="H2">
         <v>14</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1373,23 +1385,26 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3">
-        <v>2048</v>
-      </c>
+      <c r="E3" s="4"/>
       <c r="F3">
         <v>2048</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1397,23 +1412,26 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4">
+      <c r="E4" s="4"/>
+      <c r="F4">
         <v>947</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1185</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1421,23 +1439,26 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5">
-        <v>1336</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5">
         <v>1336</v>
       </c>
       <c r="G5">
+        <v>1336</v>
+      </c>
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1445,23 +1466,26 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6">
-        <v>1336</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6">
         <v>1336</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>1336</v>
       </c>
       <c r="H6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1469,23 +1493,26 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7">
+      <c r="E7" s="4"/>
+      <c r="F7">
         <v>3787</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4710</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="H7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1493,23 +1520,26 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8">
+      <c r="E8" s="4"/>
+      <c r="F8">
         <v>3789</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>4710</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>5</v>
       </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1517,23 +1547,26 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9">
-        <v>256</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9">
         <v>256</v>
       </c>
       <c r="G9">
+        <v>256</v>
+      </c>
+      <c r="H9">
         <v>99</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1541,23 +1574,26 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10">
-        <v>2048</v>
-      </c>
+      <c r="E10" s="4"/>
       <c r="F10">
         <v>2048</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1565,23 +1601,26 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11">
-        <v>2048</v>
-      </c>
+      <c r="E11" s="4"/>
       <c r="F11">
         <v>2048</v>
       </c>
       <c r="G11">
+        <v>2048</v>
+      </c>
+      <c r="H11">
         <v>14</v>
       </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1589,23 +1628,26 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12">
-        <v>2048</v>
-      </c>
+      <c r="E12" s="4"/>
       <c r="F12">
         <v>2048</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1613,23 +1655,26 @@
         <v>43</v>
       </c>
       <c r="C13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13">
-        <v>2048</v>
-      </c>
+      <c r="E13" s="4"/>
       <c r="F13">
         <v>2048</v>
       </c>
       <c r="G13">
+        <v>2048</v>
+      </c>
+      <c r="H13">
         <v>12</v>
       </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1637,23 +1682,26 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14">
-        <v>2048</v>
-      </c>
+      <c r="E14" s="4"/>
       <c r="F14">
         <v>2048</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1661,23 +1709,26 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15">
-        <v>589</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15">
         <v>589</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>589</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1685,23 +1736,26 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16">
-        <v>1860</v>
-      </c>
+      <c r="E16" s="4"/>
       <c r="F16">
         <v>1860</v>
       </c>
       <c r="G16">
+        <v>1860</v>
+      </c>
+      <c r="H16">
         <v>11</v>
       </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1709,23 +1763,26 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D17" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17">
-        <v>1860</v>
-      </c>
+      <c r="E17" s="4"/>
       <c r="F17">
         <v>1860</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>1860</v>
       </c>
       <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1733,23 +1790,26 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18">
-        <v>2048</v>
-      </c>
+      <c r="E18" s="4"/>
       <c r="F18">
         <v>2048</v>
       </c>
       <c r="G18">
+        <v>2048</v>
+      </c>
+      <c r="H18">
         <v>10</v>
       </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1757,23 +1817,26 @@
         <v>55</v>
       </c>
       <c r="C19" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19">
-        <v>1024</v>
-      </c>
+      <c r="E19" s="4"/>
       <c r="F19">
         <v>1024</v>
       </c>
       <c r="G19">
+        <v>1024</v>
+      </c>
+      <c r="H19">
         <v>16</v>
       </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1781,23 +1844,26 @@
         <v>57</v>
       </c>
       <c r="C20" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20">
-        <v>1024</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20">
         <v>1024</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>1024</v>
       </c>
       <c r="H20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1805,23 +1871,26 @@
         <v>59</v>
       </c>
       <c r="C21" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21">
-        <v>3104</v>
-      </c>
+      <c r="E21" s="4"/>
       <c r="F21">
         <v>3104</v>
       </c>
       <c r="G21">
+        <v>3104</v>
+      </c>
+      <c r="H21">
         <v>11</v>
       </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1829,23 +1898,26 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
+        <v>211</v>
+      </c>
+      <c r="D22" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22">
-        <v>3104</v>
-      </c>
+      <c r="E22" s="4"/>
       <c r="F22">
         <v>3104</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>3104</v>
       </c>
       <c r="H22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1853,23 +1925,26 @@
         <v>63</v>
       </c>
       <c r="C23" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23">
+      <c r="E23" s="4"/>
+      <c r="F23">
         <v>474</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>589</v>
       </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1877,23 +1952,26 @@
         <v>65</v>
       </c>
       <c r="C24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24">
-        <v>512</v>
-      </c>
+      <c r="E24" s="4"/>
       <c r="F24">
         <v>512</v>
       </c>
       <c r="G24">
+        <v>512</v>
+      </c>
+      <c r="H24">
         <v>60</v>
       </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1901,23 +1979,26 @@
         <v>67</v>
       </c>
       <c r="C25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D25" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25">
-        <v>512</v>
-      </c>
+      <c r="E25" s="4"/>
       <c r="F25">
         <v>512</v>
       </c>
       <c r="G25">
+        <v>512</v>
+      </c>
+      <c r="H25">
         <v>60</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1925,23 +2006,26 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26">
+      <c r="E26" s="4"/>
+      <c r="F26">
         <v>244</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>588</v>
       </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
       <c r="H26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1949,23 +2033,26 @@
         <v>71</v>
       </c>
       <c r="C27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27">
-        <v>512</v>
-      </c>
+      <c r="E27" s="4"/>
       <c r="F27">
         <v>512</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>512</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1973,23 +2060,26 @@
         <v>73</v>
       </c>
       <c r="C28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28">
-        <v>1024</v>
-      </c>
+      <c r="E28" s="4"/>
       <c r="F28">
         <v>1024</v>
       </c>
       <c r="G28">
+        <v>1024</v>
+      </c>
+      <c r="H28">
         <v>22</v>
       </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1997,23 +2087,26 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
+        <v>211</v>
+      </c>
+      <c r="D29" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29">
-        <v>1024</v>
-      </c>
+      <c r="E29" s="4"/>
       <c r="F29">
         <v>1024</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>1024</v>
       </c>
       <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2021,23 +2114,26 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D30" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30">
-        <v>1024</v>
-      </c>
+      <c r="E30" s="4"/>
       <c r="F30">
         <v>1024</v>
       </c>
       <c r="G30">
+        <v>1024</v>
+      </c>
+      <c r="H30">
         <v>28</v>
       </c>
-      <c r="H30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2045,23 +2141,26 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31">
-        <v>1024</v>
-      </c>
+      <c r="E31" s="4"/>
       <c r="F31">
         <v>1024</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>1024</v>
       </c>
       <c r="H31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2069,23 +2168,26 @@
         <v>81</v>
       </c>
       <c r="C32" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32">
+      <c r="E32" s="4"/>
+      <c r="F32">
         <v>1898</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>2816</v>
       </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
       <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2093,23 +2195,26 @@
         <v>83</v>
       </c>
       <c r="C33" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33">
-        <v>1024</v>
-      </c>
+      <c r="E33" s="4"/>
       <c r="F33">
         <v>1024</v>
       </c>
       <c r="G33">
+        <v>1024</v>
+      </c>
+      <c r="H33">
         <v>12</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2117,23 +2222,26 @@
         <v>85</v>
       </c>
       <c r="C34" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34">
+      <c r="E34" s="4"/>
+      <c r="F34">
         <v>2359</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>2362</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>5</v>
       </c>
-      <c r="H34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2141,23 +2249,26 @@
         <v>87</v>
       </c>
       <c r="C35" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35">
+      <c r="E35" s="4"/>
+      <c r="F35">
         <v>2867</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>4710</v>
       </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
       <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2165,23 +2276,26 @@
         <v>89</v>
       </c>
       <c r="C36" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36">
+      <c r="E36" s="4"/>
+      <c r="F36">
         <v>1434</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>1894</v>
       </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
       <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2189,23 +2303,26 @@
         <v>91</v>
       </c>
       <c r="C37" t="s">
+        <v>211</v>
+      </c>
+      <c r="D37" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37">
+      <c r="E37" s="4"/>
+      <c r="F37">
         <v>1894</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>3277</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
       <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2213,23 +2330,26 @@
         <v>93</v>
       </c>
       <c r="C38" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38">
-        <v>5992</v>
-      </c>
+      <c r="E38" s="4"/>
       <c r="F38">
         <v>5992</v>
       </c>
       <c r="G38">
+        <v>5992</v>
+      </c>
+      <c r="H38">
         <v>4</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2237,23 +2357,26 @@
         <v>95</v>
       </c>
       <c r="C39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D39" t="s">
         <v>96</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39">
+      <c r="E39" s="4"/>
+      <c r="F39">
         <v>4066</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>5992</v>
       </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
       <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -2261,23 +2384,26 @@
         <v>97</v>
       </c>
       <c r="C40" t="s">
+        <v>211</v>
+      </c>
+      <c r="D40" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40">
+      <c r="E40" s="4"/>
+      <c r="F40">
         <v>1437</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>2355</v>
       </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
       <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -2285,23 +2411,26 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
+        <v>211</v>
+      </c>
+      <c r="D41" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41">
-        <v>256</v>
-      </c>
+      <c r="E41" s="4"/>
       <c r="F41">
         <v>256</v>
       </c>
       <c r="G41">
+        <v>256</v>
+      </c>
+      <c r="H41">
         <v>24</v>
       </c>
-      <c r="H41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -2309,23 +2438,26 @@
         <v>101</v>
       </c>
       <c r="C42" t="s">
+        <v>211</v>
+      </c>
+      <c r="D42" t="s">
         <v>102</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42">
-        <v>256</v>
-      </c>
+      <c r="E42" s="4"/>
       <c r="F42">
         <v>256</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>256</v>
       </c>
       <c r="H42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2333,23 +2465,26 @@
         <v>103</v>
       </c>
       <c r="C43" t="s">
+        <v>211</v>
+      </c>
+      <c r="D43" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43">
-        <v>256</v>
-      </c>
+      <c r="E43" s="4"/>
       <c r="F43">
         <v>256</v>
       </c>
       <c r="G43">
+        <v>256</v>
+      </c>
+      <c r="H43">
         <v>24</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2357,23 +2492,26 @@
         <v>105</v>
       </c>
       <c r="C44" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44">
+      <c r="E44" s="4"/>
+      <c r="F44">
         <v>2354</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>2355</v>
       </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
       <c r="H44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -2381,23 +2519,26 @@
         <v>107</v>
       </c>
       <c r="C45" t="s">
+        <v>211</v>
+      </c>
+      <c r="D45" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="4"/>
-      <c r="E45">
-        <v>3440</v>
-      </c>
+      <c r="E45" s="4"/>
       <c r="F45">
         <v>3440</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>3440</v>
       </c>
       <c r="H45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2405,23 +2546,26 @@
         <v>109</v>
       </c>
       <c r="C46" t="s">
+        <v>211</v>
+      </c>
+      <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="E46">
-        <v>3440</v>
-      </c>
+      <c r="E46" s="4"/>
       <c r="F46">
         <v>3440</v>
       </c>
       <c r="G46">
+        <v>3440</v>
+      </c>
+      <c r="H46">
         <v>12</v>
       </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2429,23 +2573,26 @@
         <v>111</v>
       </c>
       <c r="C47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47">
-        <v>1893</v>
-      </c>
+      <c r="E47" s="4"/>
       <c r="F47">
         <v>1893</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>1893</v>
       </c>
       <c r="H47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2453,23 +2600,26 @@
         <v>113</v>
       </c>
       <c r="C48" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="E48">
-        <v>1893</v>
-      </c>
+      <c r="E48" s="4"/>
       <c r="F48">
         <v>1893</v>
       </c>
       <c r="G48">
+        <v>1893</v>
+      </c>
+      <c r="H48">
         <v>3</v>
       </c>
-      <c r="H48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2477,23 +2627,26 @@
         <v>115</v>
       </c>
       <c r="C49" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49">
-        <v>1648</v>
-      </c>
+      <c r="E49" s="4"/>
       <c r="F49">
         <v>1648</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>1648</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -2501,23 +2654,26 @@
         <v>117</v>
       </c>
       <c r="C50" t="s">
+        <v>211</v>
+      </c>
+      <c r="D50" t="s">
         <v>118</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50">
-        <v>1648</v>
-      </c>
+      <c r="E50" s="4"/>
       <c r="F50">
         <v>1648</v>
       </c>
       <c r="G50">
+        <v>1648</v>
+      </c>
+      <c r="H50">
         <v>11</v>
       </c>
-      <c r="H50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -2525,23 +2681,26 @@
         <v>119</v>
       </c>
       <c r="C51" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51">
-        <v>1893</v>
-      </c>
+      <c r="E51" s="4"/>
       <c r="F51">
         <v>1893</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>1893</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -2549,23 +2708,26 @@
         <v>121</v>
       </c>
       <c r="C52" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52">
-        <v>1893</v>
-      </c>
+      <c r="E52" s="4"/>
       <c r="F52">
         <v>1893</v>
       </c>
       <c r="G52">
+        <v>1893</v>
+      </c>
+      <c r="H52">
         <v>7</v>
       </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2573,23 +2735,26 @@
         <v>123</v>
       </c>
       <c r="C53" t="s">
+        <v>211</v>
+      </c>
+      <c r="D53" t="s">
         <v>124</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53">
+      <c r="E53" s="4"/>
+      <c r="F53">
         <v>1894</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>1893</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>7</v>
       </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2597,23 +2762,26 @@
         <v>125</v>
       </c>
       <c r="C54" t="s">
+        <v>211</v>
+      </c>
+      <c r="D54" t="s">
         <v>126</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54">
-        <v>512</v>
-      </c>
+      <c r="E54" s="4"/>
       <c r="F54">
         <v>512</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>512</v>
       </c>
       <c r="H54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -2621,23 +2789,26 @@
         <v>127</v>
       </c>
       <c r="C55" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="4"/>
-      <c r="E55">
-        <v>512</v>
-      </c>
+      <c r="E55" s="4"/>
       <c r="F55">
         <v>512</v>
       </c>
       <c r="G55">
+        <v>512</v>
+      </c>
+      <c r="H55">
         <v>11</v>
       </c>
-      <c r="H55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2645,23 +2816,26 @@
         <v>129</v>
       </c>
       <c r="C56" t="s">
+        <v>211</v>
+      </c>
+      <c r="D56" t="s">
         <v>130</v>
       </c>
-      <c r="D56" s="4"/>
-      <c r="E56">
-        <v>1894</v>
-      </c>
+      <c r="E56" s="4"/>
       <c r="F56">
         <v>1894</v>
       </c>
       <c r="G56">
+        <v>1894</v>
+      </c>
+      <c r="H56">
         <v>11</v>
       </c>
-      <c r="H56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2669,23 +2843,26 @@
         <v>131</v>
       </c>
       <c r="C57" t="s">
+        <v>211</v>
+      </c>
+      <c r="D57" t="s">
         <v>132</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="E57">
-        <v>946</v>
-      </c>
+      <c r="E57" s="4"/>
       <c r="F57">
         <v>946</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>946</v>
       </c>
       <c r="H57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2693,23 +2870,26 @@
         <v>133</v>
       </c>
       <c r="C58" t="s">
+        <v>211</v>
+      </c>
+      <c r="D58" t="s">
         <v>134</v>
       </c>
-      <c r="D58" s="4"/>
-      <c r="E58">
-        <v>946</v>
-      </c>
+      <c r="E58" s="4"/>
       <c r="F58">
         <v>946</v>
       </c>
       <c r="G58">
+        <v>946</v>
+      </c>
+      <c r="H58">
         <v>6</v>
       </c>
-      <c r="H58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2717,23 +2897,26 @@
         <v>135</v>
       </c>
       <c r="C59" t="s">
+        <v>211</v>
+      </c>
+      <c r="D59" t="s">
         <v>136</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59">
-        <v>946</v>
-      </c>
+      <c r="E59" s="4"/>
       <c r="F59">
         <v>946</v>
       </c>
       <c r="G59">
+        <v>946</v>
+      </c>
+      <c r="H59">
         <v>5</v>
       </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -2741,23 +2924,26 @@
         <v>137</v>
       </c>
       <c r="C60" t="s">
+        <v>211</v>
+      </c>
+      <c r="D60" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60">
-        <v>946</v>
-      </c>
+      <c r="E60" s="4"/>
       <c r="F60">
         <v>946</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>946</v>
       </c>
       <c r="H60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2765,23 +2951,26 @@
         <v>139</v>
       </c>
       <c r="C61" t="s">
+        <v>211</v>
+      </c>
+      <c r="D61" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61">
-        <v>2048</v>
-      </c>
+      <c r="E61" s="4"/>
       <c r="F61">
         <v>2048</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2789,23 +2978,26 @@
         <v>141</v>
       </c>
       <c r="C62" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="4"/>
-      <c r="E62">
-        <v>2048</v>
-      </c>
+      <c r="E62" s="4"/>
       <c r="F62">
         <v>2048</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2813,23 +3005,26 @@
         <v>143</v>
       </c>
       <c r="C63" t="s">
+        <v>211</v>
+      </c>
+      <c r="D63" t="s">
         <v>144</v>
       </c>
-      <c r="D63" s="4"/>
-      <c r="E63">
-        <v>2048</v>
-      </c>
+      <c r="E63" s="4"/>
       <c r="F63">
         <v>2048</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -2837,23 +3032,26 @@
         <v>145</v>
       </c>
       <c r="C64" t="s">
+        <v>211</v>
+      </c>
+      <c r="D64" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="4"/>
-      <c r="E64">
+      <c r="E64" s="4"/>
+      <c r="F64">
         <v>1433</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>2815</v>
       </c>
-      <c r="G64">
-        <v>1</v>
-      </c>
       <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -2861,23 +3059,26 @@
         <v>147</v>
       </c>
       <c r="C65" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" t="s">
         <v>148</v>
       </c>
-      <c r="D65" s="4"/>
-      <c r="E65">
+      <c r="E65" s="4"/>
+      <c r="F65">
         <v>1433</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>2815</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>13</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -2885,23 +3086,26 @@
         <v>149</v>
       </c>
       <c r="C66" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="4"/>
-      <c r="E66">
-        <v>2048</v>
-      </c>
+      <c r="E66" s="4"/>
       <c r="F66">
         <v>2048</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -2909,23 +3113,26 @@
         <v>151</v>
       </c>
       <c r="C67" t="s">
+        <v>211</v>
+      </c>
+      <c r="D67" t="s">
         <v>152</v>
       </c>
-      <c r="D67" s="4"/>
-      <c r="E67">
-        <v>2048</v>
-      </c>
+      <c r="E67" s="4"/>
       <c r="F67">
         <v>2048</v>
       </c>
       <c r="G67">
+        <v>2048</v>
+      </c>
+      <c r="H67">
         <v>78</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -2933,23 +3140,26 @@
         <v>153</v>
       </c>
       <c r="C68" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" t="s">
         <v>154</v>
       </c>
-      <c r="D68" s="4"/>
-      <c r="E68">
+      <c r="E68" s="4"/>
+      <c r="F68">
         <v>5733</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>9420</v>
       </c>
-      <c r="G68">
-        <v>1</v>
-      </c>
       <c r="H68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -2957,23 +3167,26 @@
         <v>155</v>
       </c>
       <c r="C69" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" t="s">
         <v>156</v>
       </c>
-      <c r="D69" s="4"/>
-      <c r="E69">
+      <c r="E69" s="4"/>
+      <c r="F69">
         <v>5733</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>9420</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>9</v>
       </c>
-      <c r="H69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -2981,23 +3194,26 @@
         <v>157</v>
       </c>
       <c r="C70" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" t="s">
         <v>158</v>
       </c>
-      <c r="D70" s="4"/>
-      <c r="E70">
+      <c r="E70" s="4"/>
+      <c r="F70">
         <v>5733</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>9420</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>4</v>
       </c>
-      <c r="H70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -3005,23 +3221,26 @@
         <v>159</v>
       </c>
       <c r="C71" t="s">
+        <v>211</v>
+      </c>
+      <c r="D71" t="s">
         <v>160</v>
       </c>
-      <c r="D71" s="4"/>
-      <c r="E71">
-        <v>2048</v>
-      </c>
+      <c r="E71" s="4"/>
       <c r="F71">
         <v>2048</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>2048</v>
       </c>
       <c r="H71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -3029,23 +3248,26 @@
         <v>161</v>
       </c>
       <c r="C72" t="s">
+        <v>211</v>
+      </c>
+      <c r="D72" t="s">
         <v>162</v>
       </c>
-      <c r="D72" s="4"/>
-      <c r="E72">
+      <c r="E72" s="4"/>
+      <c r="F72">
         <v>4065</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>7917</v>
       </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
       <c r="H72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -3053,23 +3275,26 @@
         <v>163</v>
       </c>
       <c r="C73" t="s">
+        <v>211</v>
+      </c>
+      <c r="D73" t="s">
         <v>164</v>
       </c>
-      <c r="D73" s="4"/>
-      <c r="E73">
+      <c r="E73" s="4"/>
+      <c r="F73">
         <v>4065</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>7917</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>9</v>
       </c>
-      <c r="H73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -3077,23 +3302,26 @@
         <v>165</v>
       </c>
       <c r="C74" t="s">
+        <v>211</v>
+      </c>
+      <c r="D74" t="s">
         <v>166</v>
       </c>
-      <c r="D74" s="4"/>
-      <c r="E74">
+      <c r="E74" s="4"/>
+      <c r="F74">
         <v>1433</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>1894</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>10</v>
       </c>
-      <c r="H74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -3101,23 +3329,26 @@
         <v>167</v>
       </c>
       <c r="C75" t="s">
+        <v>211</v>
+      </c>
+      <c r="D75" t="s">
         <v>168</v>
       </c>
-      <c r="D75" s="4"/>
-      <c r="E75">
+      <c r="E75" s="4"/>
+      <c r="F75">
         <v>1433</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>1894</v>
       </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
       <c r="H75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -3125,23 +3356,26 @@
         <v>169</v>
       </c>
       <c r="C76" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" t="s">
         <v>170</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76">
+      <c r="E76" s="4"/>
+      <c r="F76">
         <v>4065</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>7917</v>
       </c>
-      <c r="G76">
-        <v>1</v>
-      </c>
       <c r="H76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3149,23 +3383,26 @@
         <v>171</v>
       </c>
       <c r="C77" t="s">
+        <v>211</v>
+      </c>
+      <c r="D77" t="s">
         <v>172</v>
       </c>
-      <c r="D77" s="4"/>
-      <c r="E77">
+      <c r="E77" s="4"/>
+      <c r="F77">
         <v>4065</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>7917</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>12</v>
       </c>
-      <c r="H77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -3173,23 +3410,26 @@
         <v>173</v>
       </c>
       <c r="C78" t="s">
+        <v>211</v>
+      </c>
+      <c r="D78" t="s">
         <v>174</v>
       </c>
-      <c r="D78" s="4"/>
-      <c r="E78">
-        <v>512</v>
-      </c>
+      <c r="E78" s="4"/>
       <c r="F78">
         <v>512</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>512</v>
       </c>
       <c r="H78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3197,23 +3437,26 @@
         <v>175</v>
       </c>
       <c r="C79" t="s">
+        <v>211</v>
+      </c>
+      <c r="D79" t="s">
         <v>176</v>
       </c>
-      <c r="D79" s="4"/>
-      <c r="E79">
-        <v>1024</v>
-      </c>
+      <c r="E79" s="4"/>
       <c r="F79">
         <v>1024</v>
       </c>
       <c r="G79">
+        <v>1024</v>
+      </c>
+      <c r="H79">
         <v>47</v>
       </c>
-      <c r="H79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -3221,23 +3464,26 @@
         <v>177</v>
       </c>
       <c r="C80" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" t="s">
         <v>178</v>
       </c>
-      <c r="D80" s="4"/>
-      <c r="E80">
-        <v>1656</v>
-      </c>
+      <c r="E80" s="4"/>
       <c r="F80">
         <v>1656</v>
       </c>
       <c r="G80">
+        <v>1656</v>
+      </c>
+      <c r="H80">
         <v>68</v>
       </c>
-      <c r="H80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -3245,23 +3491,26 @@
         <v>179</v>
       </c>
       <c r="C81" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" t="s">
         <v>180</v>
       </c>
-      <c r="D81" s="4"/>
-      <c r="E81">
+      <c r="E81" s="4"/>
+      <c r="F81">
         <v>1407</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>1177</v>
       </c>
-      <c r="G81">
-        <v>1</v>
-      </c>
       <c r="H81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -3269,23 +3518,26 @@
         <v>181</v>
       </c>
       <c r="C82" t="s">
+        <v>211</v>
+      </c>
+      <c r="D82" t="s">
         <v>182</v>
       </c>
-      <c r="D82" s="4"/>
-      <c r="E82">
-        <v>1648</v>
-      </c>
+      <c r="E82" s="4"/>
       <c r="F82">
         <v>1648</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>1648</v>
       </c>
       <c r="H82">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -3293,23 +3545,26 @@
         <v>183</v>
       </c>
       <c r="C83" t="s">
+        <v>211</v>
+      </c>
+      <c r="D83" t="s">
         <v>184</v>
       </c>
-      <c r="D83" s="4"/>
-      <c r="E83">
+      <c r="E83" s="4"/>
+      <c r="F83">
         <v>1407</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>1177</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>11</v>
       </c>
-      <c r="H83">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -3317,23 +3572,26 @@
         <v>185</v>
       </c>
       <c r="C84" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" t="s">
         <v>186</v>
       </c>
-      <c r="D84" s="4"/>
-      <c r="E84">
-        <v>1648</v>
-      </c>
+      <c r="E84" s="4"/>
       <c r="F84">
         <v>1648</v>
       </c>
       <c r="G84">
+        <v>1648</v>
+      </c>
+      <c r="H84">
         <v>8</v>
       </c>
-      <c r="H84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -3341,23 +3599,26 @@
         <v>187</v>
       </c>
       <c r="C85" t="s">
+        <v>211</v>
+      </c>
+      <c r="D85" t="s">
         <v>188</v>
       </c>
-      <c r="D85" s="4"/>
-      <c r="E85">
+      <c r="E85" s="4"/>
+      <c r="F85">
         <v>9063</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>7580</v>
       </c>
-      <c r="G85">
-        <v>1</v>
-      </c>
       <c r="H85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -3365,23 +3626,26 @@
         <v>189</v>
       </c>
       <c r="C86" t="s">
+        <v>211</v>
+      </c>
+      <c r="D86" t="s">
         <v>190</v>
       </c>
-      <c r="D86" s="4"/>
-      <c r="E86">
+      <c r="E86" s="4"/>
+      <c r="F86">
         <v>9063</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>7580</v>
       </c>
-      <c r="G86">
-        <v>1</v>
-      </c>
       <c r="H86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -3389,23 +3653,26 @@
         <v>191</v>
       </c>
       <c r="C87" t="s">
+        <v>211</v>
+      </c>
+      <c r="D87" t="s">
         <v>192</v>
       </c>
-      <c r="D87" s="4"/>
-      <c r="E87">
-        <v>2200</v>
-      </c>
+      <c r="E87" s="4"/>
       <c r="F87">
         <v>2200</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>2200</v>
       </c>
       <c r="H87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -3413,23 +3680,26 @@
         <v>193</v>
       </c>
       <c r="C88" t="s">
+        <v>211</v>
+      </c>
+      <c r="D88" t="s">
         <v>194</v>
       </c>
-      <c r="D88" s="4"/>
-      <c r="E88">
-        <v>2200</v>
-      </c>
+      <c r="E88" s="4"/>
       <c r="F88">
         <v>2200</v>
       </c>
       <c r="G88">
+        <v>2200</v>
+      </c>
+      <c r="H88">
         <v>12</v>
       </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -3437,23 +3707,26 @@
         <v>195</v>
       </c>
       <c r="C89" t="s">
+        <v>211</v>
+      </c>
+      <c r="D89" t="s">
         <v>196</v>
       </c>
-      <c r="D89" s="4"/>
-      <c r="E89">
+      <c r="E89" s="4"/>
+      <c r="F89">
         <v>2354</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>1894</v>
       </c>
-      <c r="G89">
-        <v>1</v>
-      </c>
       <c r="H89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>17</v>
       </c>
@@ -3461,25 +3734,28 @@
         <v>197</v>
       </c>
       <c r="C90" t="s">
+        <v>211</v>
+      </c>
+      <c r="D90" t="s">
         <v>198</v>
       </c>
-      <c r="D90" s="4"/>
-      <c r="E90">
+      <c r="E90" s="4"/>
+      <c r="F90">
         <v>2354</v>
       </c>
-      <c r="F90">
+      <c r="G90">
         <v>1894</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>9</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:D90"/>
+    <mergeCell ref="E2:E90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update block metadata csv
</commit_message>
<xml_diff>
--- a/config_portal/examples/images-example.xlsx
+++ b/config_portal/examples/images-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/HuBMAP-pancreas-data-explorer/HuBMAP-pancreas-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E499C9-D78E-724D-95DF-A4C6AB75045F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BE3381-BEDC-1B4F-9552-6F7D4E7BF666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
+    <workbookView xWindow="440" yWindow="2100" windowWidth="28040" windowHeight="17440" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
   </bookViews>
   <sheets>
     <sheet name="block-data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="216">
   <si>
     <t>Order</t>
   </si>
@@ -636,9 +636,6 @@
     <t>P2-7A TH 633.czi</t>
   </si>
   <si>
-    <t>Organ</t>
-  </si>
-  <si>
     <t>Change values to T/F and auto-generate links</t>
   </si>
   <si>
@@ -676,6 +673,18 @@
   </si>
   <si>
     <t>Image Category</t>
+  </si>
+  <si>
+    <t>Organ ID</t>
+  </si>
+  <si>
+    <t>Organ Description</t>
+  </si>
+  <si>
+    <t>Pancreas 1</t>
+  </si>
+  <si>
+    <t>Pancreas 2</t>
   </si>
 </sst>
 </file>
@@ -1075,235 +1084,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989D2757-BD7C-144B-BDA6-C7A7A489E518}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="6.1640625" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:G12"/>
+    <mergeCell ref="F2:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1313,7 +1361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A62E87D-1C39-EA44-B778-5ACEBBC062C4}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1321,31 +1369,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1356,13 +1404,13 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F2">
         <v>2048</v>
@@ -1385,7 +1433,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -1412,7 +1460,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -1439,7 +1487,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
@@ -1466,7 +1514,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
@@ -1493,7 +1541,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -1520,7 +1568,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -1547,7 +1595,7 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -1574,7 +1622,7 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D10" t="s">
         <v>38</v>
@@ -1601,7 +1649,7 @@
         <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -1628,7 +1676,7 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
@@ -1655,7 +1703,7 @@
         <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D13" t="s">
         <v>44</v>
@@ -1682,7 +1730,7 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -1709,7 +1757,7 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D15" t="s">
         <v>48</v>
@@ -1736,7 +1784,7 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" t="s">
         <v>50</v>
@@ -1763,7 +1811,7 @@
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D17" t="s">
         <v>52</v>
@@ -1790,7 +1838,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D18" t="s">
         <v>54</v>
@@ -1817,7 +1865,7 @@
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" t="s">
         <v>56</v>
@@ -1844,7 +1892,7 @@
         <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D20" t="s">
         <v>58</v>
@@ -1871,7 +1919,7 @@
         <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D21" t="s">
         <v>60</v>
@@ -1898,7 +1946,7 @@
         <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D22" t="s">
         <v>62</v>
@@ -1925,7 +1973,7 @@
         <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D23" t="s">
         <v>64</v>
@@ -1952,7 +2000,7 @@
         <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D24" t="s">
         <v>66</v>
@@ -1979,7 +2027,7 @@
         <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D25" t="s">
         <v>68</v>
@@ -2006,7 +2054,7 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D26" t="s">
         <v>70</v>
@@ -2033,7 +2081,7 @@
         <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D27" t="s">
         <v>72</v>
@@ -2060,7 +2108,7 @@
         <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D28" t="s">
         <v>74</v>
@@ -2087,7 +2135,7 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D29" t="s">
         <v>76</v>
@@ -2114,7 +2162,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D30" t="s">
         <v>78</v>
@@ -2141,7 +2189,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D31" t="s">
         <v>80</v>
@@ -2168,7 +2216,7 @@
         <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D32" t="s">
         <v>82</v>
@@ -2195,7 +2243,7 @@
         <v>83</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D33" t="s">
         <v>84</v>
@@ -2222,7 +2270,7 @@
         <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D34" t="s">
         <v>86</v>
@@ -2249,7 +2297,7 @@
         <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D35" t="s">
         <v>88</v>
@@ -2276,7 +2324,7 @@
         <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D36" t="s">
         <v>90</v>
@@ -2303,7 +2351,7 @@
         <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D37" t="s">
         <v>92</v>
@@ -2330,7 +2378,7 @@
         <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D38" t="s">
         <v>94</v>
@@ -2357,7 +2405,7 @@
         <v>95</v>
       </c>
       <c r="C39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D39" t="s">
         <v>96</v>
@@ -2384,7 +2432,7 @@
         <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D40" t="s">
         <v>98</v>
@@ -2411,7 +2459,7 @@
         <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D41" t="s">
         <v>100</v>
@@ -2438,7 +2486,7 @@
         <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D42" t="s">
         <v>102</v>
@@ -2465,7 +2513,7 @@
         <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D43" t="s">
         <v>104</v>
@@ -2492,7 +2540,7 @@
         <v>105</v>
       </c>
       <c r="C44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D44" t="s">
         <v>106</v>
@@ -2519,7 +2567,7 @@
         <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D45" t="s">
         <v>108</v>
@@ -2546,7 +2594,7 @@
         <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D46" t="s">
         <v>110</v>
@@ -2573,7 +2621,7 @@
         <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D47" t="s">
         <v>112</v>
@@ -2600,7 +2648,7 @@
         <v>113</v>
       </c>
       <c r="C48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D48" t="s">
         <v>114</v>
@@ -2627,7 +2675,7 @@
         <v>115</v>
       </c>
       <c r="C49" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D49" t="s">
         <v>116</v>
@@ -2654,7 +2702,7 @@
         <v>117</v>
       </c>
       <c r="C50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D50" t="s">
         <v>118</v>
@@ -2681,7 +2729,7 @@
         <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D51" t="s">
         <v>120</v>
@@ -2708,7 +2756,7 @@
         <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D52" t="s">
         <v>122</v>
@@ -2735,7 +2783,7 @@
         <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D53" t="s">
         <v>124</v>
@@ -2762,7 +2810,7 @@
         <v>125</v>
       </c>
       <c r="C54" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D54" t="s">
         <v>126</v>
@@ -2789,7 +2837,7 @@
         <v>127</v>
       </c>
       <c r="C55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D55" t="s">
         <v>128</v>
@@ -2816,7 +2864,7 @@
         <v>129</v>
       </c>
       <c r="C56" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D56" t="s">
         <v>130</v>
@@ -2843,7 +2891,7 @@
         <v>131</v>
       </c>
       <c r="C57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D57" t="s">
         <v>132</v>
@@ -2870,7 +2918,7 @@
         <v>133</v>
       </c>
       <c r="C58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D58" t="s">
         <v>134</v>
@@ -2897,7 +2945,7 @@
         <v>135</v>
       </c>
       <c r="C59" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D59" t="s">
         <v>136</v>
@@ -2924,7 +2972,7 @@
         <v>137</v>
       </c>
       <c r="C60" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D60" t="s">
         <v>138</v>
@@ -2951,7 +2999,7 @@
         <v>139</v>
       </c>
       <c r="C61" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D61" t="s">
         <v>140</v>
@@ -2978,7 +3026,7 @@
         <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D62" t="s">
         <v>142</v>
@@ -3005,7 +3053,7 @@
         <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D63" t="s">
         <v>144</v>
@@ -3032,7 +3080,7 @@
         <v>145</v>
       </c>
       <c r="C64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D64" t="s">
         <v>146</v>
@@ -3059,7 +3107,7 @@
         <v>147</v>
       </c>
       <c r="C65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D65" t="s">
         <v>148</v>
@@ -3086,7 +3134,7 @@
         <v>149</v>
       </c>
       <c r="C66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D66" t="s">
         <v>150</v>
@@ -3113,7 +3161,7 @@
         <v>151</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D67" t="s">
         <v>152</v>
@@ -3140,7 +3188,7 @@
         <v>153</v>
       </c>
       <c r="C68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D68" t="s">
         <v>154</v>
@@ -3167,7 +3215,7 @@
         <v>155</v>
       </c>
       <c r="C69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s">
         <v>156</v>
@@ -3194,7 +3242,7 @@
         <v>157</v>
       </c>
       <c r="C70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D70" t="s">
         <v>158</v>
@@ -3221,7 +3269,7 @@
         <v>159</v>
       </c>
       <c r="C71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D71" t="s">
         <v>160</v>
@@ -3248,7 +3296,7 @@
         <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D72" t="s">
         <v>162</v>
@@ -3275,7 +3323,7 @@
         <v>163</v>
       </c>
       <c r="C73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D73" t="s">
         <v>164</v>
@@ -3302,7 +3350,7 @@
         <v>165</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D74" t="s">
         <v>166</v>
@@ -3329,7 +3377,7 @@
         <v>167</v>
       </c>
       <c r="C75" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D75" t="s">
         <v>168</v>
@@ -3356,7 +3404,7 @@
         <v>169</v>
       </c>
       <c r="C76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D76" t="s">
         <v>170</v>
@@ -3383,7 +3431,7 @@
         <v>171</v>
       </c>
       <c r="C77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D77" t="s">
         <v>172</v>
@@ -3410,7 +3458,7 @@
         <v>173</v>
       </c>
       <c r="C78" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D78" t="s">
         <v>174</v>
@@ -3437,7 +3485,7 @@
         <v>175</v>
       </c>
       <c r="C79" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D79" t="s">
         <v>176</v>
@@ -3464,7 +3512,7 @@
         <v>177</v>
       </c>
       <c r="C80" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D80" t="s">
         <v>178</v>
@@ -3491,7 +3539,7 @@
         <v>179</v>
       </c>
       <c r="C81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
         <v>180</v>
@@ -3518,7 +3566,7 @@
         <v>181</v>
       </c>
       <c r="C82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D82" t="s">
         <v>182</v>
@@ -3545,7 +3593,7 @@
         <v>183</v>
       </c>
       <c r="C83" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D83" t="s">
         <v>184</v>
@@ -3572,7 +3620,7 @@
         <v>185</v>
       </c>
       <c r="C84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D84" t="s">
         <v>186</v>
@@ -3599,7 +3647,7 @@
         <v>187</v>
       </c>
       <c r="C85" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D85" t="s">
         <v>188</v>
@@ -3626,7 +3674,7 @@
         <v>189</v>
       </c>
       <c r="C86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D86" t="s">
         <v>190</v>
@@ -3653,7 +3701,7 @@
         <v>191</v>
       </c>
       <c r="C87" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D87" t="s">
         <v>192</v>
@@ -3680,7 +3728,7 @@
         <v>193</v>
       </c>
       <c r="C88" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D88" t="s">
         <v>194</v>
@@ -3707,7 +3755,7 @@
         <v>195</v>
       </c>
       <c r="C89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D89" t="s">
         <v>196</v>
@@ -3734,7 +3782,7 @@
         <v>197</v>
       </c>
       <c r="C90" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D90" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
finish v1 of spatial map data update
</commit_message>
<xml_diff>
--- a/config_portal/examples/images-example.xlsx
+++ b/config_portal/examples/images-example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlabyer/Projects/HuBMAP-pancreas-data-explorer/HuBMAP-pancreas-data-explorer/config_portal/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1644F875-430A-C74E-899C-339268BE1E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052B6561-E8A2-D64D-A73A-66D5C735EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="2100" windowWidth="28040" windowHeight="17440" xr2:uid="{4C3CEB32-934F-4741-97EE-11231D60B5A9}"/>
   </bookViews>
@@ -682,7 +682,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -693,6 +693,7 @@
     <font>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1059,10 +1060,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
@@ -1073,7 +1074,7 @@
     <col min="8" max="8" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1122,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1138,12 +1139,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2" t="b">
-        <v>1</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1161,11 +1160,8 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1181,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1205,7 +1201,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1223,9 +1219,11 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="H7" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1245,7 +1243,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1265,7 +1263,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1285,7 +1283,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1305,7 +1303,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1338,9 +1336,9 @@
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
@@ -1366,7 +1364,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1392,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1418,7 +1416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1444,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1470,7 +1468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1496,7 +1494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1522,7 +1520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1548,7 +1546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1574,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1600,7 +1598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1626,7 +1624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1678,7 +1676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1730,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1756,7 +1754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1782,7 +1780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1808,7 +1806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1834,7 +1832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1860,7 +1858,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1886,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1912,7 +1910,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1938,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2016,7 +2014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -2042,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2068,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -2120,7 +2118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -2146,7 +2144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -2172,7 +2170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -2198,7 +2196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2224,7 +2222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -2250,7 +2248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2276,7 +2274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -2302,7 +2300,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -2328,7 +2326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2354,7 +2352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +2378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -2406,7 +2404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -2432,7 +2430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -2458,7 +2456,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -2484,7 +2482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -2510,7 +2508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2536,7 +2534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2562,7 +2560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -2588,7 +2586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -2614,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -2640,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -2666,7 +2664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -2692,7 +2690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2718,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2744,7 +2742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>18</v>
       </c>
@@ -2770,7 +2768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2796,7 +2794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>18</v>
       </c>
@@ -2822,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -2848,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -2874,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -2900,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -2926,7 +2924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -2952,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -2978,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -3004,7 +3002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>19</v>
       </c>
@@ -3030,7 +3028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>19</v>
       </c>
@@ -3056,7 +3054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>19</v>
       </c>
@@ -3082,7 +3080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>19</v>
       </c>
@@ -3108,7 +3106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -3134,7 +3132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -3160,7 +3158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -3186,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -3212,7 +3210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -3238,7 +3236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -3264,7 +3262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -3290,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -3316,7 +3314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3342,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>17</v>
       </c>
@@ -3368,7 +3366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3394,7 +3392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -3420,7 +3418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -3446,7 +3444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -3472,7 +3470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -3498,7 +3496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -3524,7 +3522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -3550,7 +3548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -3576,7 +3574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -3602,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -3628,7 +3626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -3654,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>17</v>
       </c>

</xml_diff>